<commit_message>
we unstage two files
</commit_message>
<xml_diff>
--- a/project.xlsx
+++ b/project.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>sd</t>
   </si>
@@ -359,7 +359,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -370,6 +370,9 @@
       </c>
     </row>
     <row r="11" spans="1:7">
+      <c r="F11" t="s">
+        <v>1</v>
+      </c>
       <c r="G11" t="s">
         <v>1</v>
       </c>

</xml_diff>